<commit_message>
Change pattern for cities table
</commit_message>
<xml_diff>
--- a/excelReader/zones/Zones.xlsx
+++ b/excelReader/zones/Zones.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Номер зоны</t>
   </si>
@@ -389,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -522,6 +522,23 @@
         <v>50</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>790</v>
+      </c>
+      <c r="D8" s="1">
+        <v>890</v>
+      </c>
+      <c r="E8" s="1">
+        <v>140</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>